<commit_message>
add test for factorial in hw 2
</commit_message>
<xml_diff>
--- a/TestCase_01.xlsx
+++ b/TestCase_01.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egor\PycharmProjects\module_4_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB620A7C-ABD8-4BAD-8169-05BDD6408783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD565B56-1DDB-40FD-88A0-984EF9F66D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="13875" windowHeight="15585" xr2:uid="{70A58EB9-CB34-46B8-8AC4-776AF9D22DEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{70A58EB9-CB34-46B8-8AC4-776AF9D22DEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="86">
   <si>
     <t>ID</t>
   </si>
@@ -163,13 +164,133 @@
   </si>
   <si>
     <t>6 Г</t>
+  </si>
+  <si>
+    <t>TypeError</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>Корректность нахождения факториала</t>
+  </si>
+  <si>
+    <t>8 П</t>
+  </si>
+  <si>
+    <t>Проверка работы функции со списком дробных чисел</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать список с дробными числами</t>
+  </si>
+  <si>
+    <t>9 П</t>
+  </si>
+  <si>
+    <t>Проверка работы функции со списком дробных и целых чисел</t>
+  </si>
+  <si>
+    <t>[1.5, 5.2, 6.42, -7.6]</t>
+  </si>
+  <si>
+    <t>[1, 5.3, -5, -6.32]</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать список с дробными и целыми числами</t>
+  </si>
+  <si>
+    <t>1.38</t>
+  </si>
+  <si>
+    <t>-1,255</t>
+  </si>
+  <si>
+    <t>-1.2550000000000001</t>
+  </si>
+  <si>
+    <t>1.3800000000000003</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Обработка некорректных входных данных</t>
+  </si>
+  <si>
+    <t>Проверка работы функции с целыми числами</t>
+  </si>
+  <si>
+    <t>Проверка работы функции с дробными числами</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>3628800</t>
+  </si>
+  <si>
+    <t>2 Н</t>
+  </si>
+  <si>
+    <t>3 Г</t>
+  </si>
+  <si>
+    <t>Проверка работы функции с 0</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать дробное число</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать положительное число</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать 0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>4 Н</t>
+  </si>
+  <si>
+    <t>Проверка работы функции типом данных str</t>
+  </si>
+  <si>
+    <t>"5"</t>
+  </si>
+  <si>
+    <t>Проверка работы функции большими числами</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>6 Н</t>
+  </si>
+  <si>
+    <t>Проверка работы функции с отрицательными числами</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать большое число</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать отрицательное число</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +298,20 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF800000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -199,9 +334,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -209,17 +343,38 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -534,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB252D5B-2D38-4C73-8A7D-EAA8C92AAD67}">
-  <dimension ref="B2:I24"/>
+  <dimension ref="B2:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,130 +706,138 @@
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="H11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="H12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="H13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -683,20 +846,22 @@
       <c r="D14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="H14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -705,20 +870,24 @@
       <c r="D15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="H15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -727,109 +896,147 @@
       <c r="D16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="9">
         <v>68</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="H16" s="9">
+        <v>68</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="2:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="H17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="8"/>
+    </row>
+    <row r="18" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -840,4 +1047,397 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967A0E80-4F8A-4AA0-81BE-B2C298CCB157}">
+  <dimension ref="B2:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="4">
+        <v>10</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G14" s="15">
+        <v>3.04140932017133E+64</v>
+      </c>
+      <c r="H14" s="15">
+        <v>3.04140932017133E+64</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>